<commit_message>
feat: added ref_id, external_ref tag for fare_pplociy & on_status call
</commit_message>
<xml_diff>
--- a/api/components/attributes/on-demand_attributes_updated.xlsx
+++ b/api/components/attributes/on-demand_attributes_updated.xlsx
@@ -8888,7 +8888,7 @@
         <v>325</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>8</v>
@@ -8968,7 +8968,7 @@
         <v>305</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>8</v>
@@ -8988,7 +8988,7 @@
         <v>307</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>8</v>
@@ -9028,7 +9028,7 @@
         <v>309</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>8</v>
@@ -9907,8 +9907,8 @@
       <c r="A73" s="21" t="s">
         <v>343</v>
       </c>
-      <c r="B73" s="18" t="s">
-        <v>60</v>
+      <c r="B73" s="21" t="s">
+        <v>50</v>
       </c>
       <c r="C73" s="17" t="s">
         <v>61</v>
@@ -9927,8 +9927,8 @@
       <c r="A74" s="7" t="s">
         <v>345</v>
       </c>
-      <c r="B74" s="18" t="s">
-        <v>60</v>
+      <c r="B74" s="21" t="s">
+        <v>50</v>
       </c>
       <c r="C74" s="17" t="s">
         <v>61</v>
@@ -9947,8 +9947,8 @@
       <c r="A75" s="7" t="s">
         <v>347</v>
       </c>
-      <c r="B75" s="18" t="s">
-        <v>60</v>
+      <c r="B75" s="21" t="s">
+        <v>50</v>
       </c>
       <c r="C75" s="17" t="s">
         <v>61</v>
@@ -10027,8 +10027,8 @@
       <c r="A79" s="7" t="s">
         <v>349</v>
       </c>
-      <c r="B79" s="18" t="s">
-        <v>60</v>
+      <c r="B79" s="21" t="s">
+        <v>50</v>
       </c>
       <c r="C79" s="17" t="s">
         <v>61</v>

</xml_diff>